<commit_message>
Fixed excel and logo
</commit_message>
<xml_diff>
--- a/Excel/Statisztika.xlsx
+++ b/Excel/Statisztika.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\PleaseHold\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17B8EBD-D0B4-4606-9792-C2B29592B720}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA064258-31D8-44A7-B957-09A036235B03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="869" activeTab="6" xr2:uid="{CBEB8FAB-31F6-424B-A567-FFE90715BD13}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="869" activeTab="4" xr2:uid="{CBEB8FAB-31F6-424B-A567-FFE90715BD13}"/>
   </bookViews>
   <sheets>
     <sheet name="Lakosok" sheetId="5" r:id="rId1"/>
@@ -24,8 +24,6 @@
   <definedNames>
     <definedName name="_xlchart.v2.0" hidden="1">'Projekt költségek'!$G$2:$G$9</definedName>
     <definedName name="_xlchart.v2.1" hidden="1">'Projekt költségek'!$H$2:$H$9</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'Projekt költségek'!$G$2:$G$9</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'Projekt költségek'!$H$2:$H$9</definedName>
     <definedName name="KülsőAdatok_1" localSheetId="3" hidden="1">'Épület projekt kapcsolótábla'!$A$1:$C$13</definedName>
     <definedName name="KülsőAdatok_1" localSheetId="1" hidden="1">Épületek!$A$1:$E$26</definedName>
     <definedName name="KülsőAdatok_1" localSheetId="0" hidden="1">Lakosok!$A$1:$E$39</definedName>
@@ -538,10 +536,10 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -560,6 +558,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -594,7 +660,7 @@
             <a:pPr>
               <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:sysClr val="windowText" lastClr="E0E0E0"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -627,7 +693,7 @@
           <a:pPr>
             <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:sysClr val="windowText" lastClr="E0E0E0"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -696,7 +762,7 @@
                 <a:pPr>
                   <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
+                      <a:sysClr val="windowText" lastClr="E0E0E0"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -849,7 +915,7 @@
             <a:pPr>
               <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:sysClr val="windowText" lastClr="E0E0E0"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -891,7 +957,7 @@
             <a:pPr>
               <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:sysClr val="windowText" lastClr="E0E0E0"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -946,7 +1012,7 @@
       <a:pPr>
         <a:defRPr sz="1100">
           <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
+            <a:sysClr val="windowText" lastClr="E0E0E0"/>
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
@@ -2374,7 +2440,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:sysClr val="window" lastClr="FFFFFF"/>
+      <a:sysClr val="window" lastClr="202020"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -3027,7 +3093,7 @@
             </c:dLbl>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
+                <a:sysClr val="window" lastClr="202020">
                   <a:alpha val="90000"/>
                 </a:sysClr>
               </a:solidFill>
@@ -3367,13 +3433,13 @@
             <c:spPr>
               <a:pattFill prst="pct75">
                 <a:fgClr>
-                  <a:sysClr val="windowText" lastClr="000000">
+                  <a:sysClr val="windowText" lastClr="E0E0E0">
                     <a:lumMod val="75000"/>
                     <a:lumOff val="25000"/>
                   </a:sysClr>
                 </a:fgClr>
                 <a:bgClr>
-                  <a:sysClr val="windowText" lastClr="000000">
+                  <a:sysClr val="windowText" lastClr="E0E0E0">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
@@ -3618,10 +3684,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v2.2</cx:f>
+        <cx:f>_xlchart.v2.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v2.3</cx:f>
+        <cx:f>_xlchart.v2.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -3677,13 +3743,13 @@
             <a:pPr algn="ctr" rtl="0">
               <a:defRPr sz="1800">
                 <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000"/>
+                  <a:sysClr val="windowText" lastClr="E0E0E0"/>
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="hu-HU" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
               <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
+                <a:sysClr val="windowText" lastClr="E0E0E0"/>
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:endParaRPr>
@@ -7755,7 +7821,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
+                <a:rPr lang="en-US" sz="1100"/>
                 <a:t>Ez a diagram nem érhető el az Excel ezen verziójában.
 Ha szerkeszti ezt az alakzatot, vagy más formátumba menti a munkafüzetet, azzal végleg tönkreteszi a diagramot.</a:t>
               </a:r>
@@ -8075,10 +8141,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="E0E0E0"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="202020"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -9813,8 +9879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A56C3A-4BBC-489F-B53E-C40E949EC3CF}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="B1 D1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9878,7 +9944,7 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <f t="array" ref="G2">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A1))), "")</f>
+        <f t="array" ref="G2">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A1))), "")</f>
         <v>iskola</v>
       </c>
       <c r="H2" s="10">
@@ -9913,7 +9979,7 @@
         <v>1000000</v>
       </c>
       <c r="G3" t="str">
-        <f t="array" ref="G3">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A2))), "")</f>
+        <f t="array" ref="G3">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A2))), "")</f>
         <v>szórakozás</v>
       </c>
       <c r="H3" s="10">
@@ -9948,7 +10014,7 @@
         <v>1000000</v>
       </c>
       <c r="G4" t="str">
-        <f t="array" ref="G4">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A3))), "")</f>
+        <f t="array" ref="G4">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A3))), "")</f>
         <v>iskola</v>
       </c>
       <c r="H4" s="10">
@@ -9983,7 +10049,7 @@
         <v/>
       </c>
       <c r="G5" t="str">
-        <f t="array" ref="G5">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A4))), "")</f>
+        <f t="array" ref="G5">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A4))), "")</f>
         <v>szórakozás</v>
       </c>
       <c r="H5" s="10">
@@ -10018,7 +10084,7 @@
         <v>2345670</v>
       </c>
       <c r="G6" t="str">
-        <f t="array" ref="G6">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A5))), "")</f>
+        <f t="array" ref="G6">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A5))), "")</f>
         <v>kulturális</v>
       </c>
       <c r="H6" s="10">
@@ -10053,7 +10119,7 @@
         <v/>
       </c>
       <c r="G7" t="str">
-        <f t="array" ref="G7">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A6))), "")</f>
+        <f t="array" ref="G7">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A6))), "")</f>
         <v>kórház</v>
       </c>
       <c r="H7" s="10">
@@ -10087,7 +10153,7 @@
         <v>576400</v>
       </c>
       <c r="G8" t="str">
-        <f t="array" ref="G8">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A7))), "")</f>
+        <f t="array" ref="G8">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A7))), "")</f>
         <v>üzlet</v>
       </c>
       <c r="H8" s="10">
@@ -10121,7 +10187,7 @@
         <v>15000000</v>
       </c>
       <c r="G9" t="str">
-        <f t="array" ref="G9">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A8))), "")</f>
+        <f t="array" ref="G9">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A8))), "")</f>
         <v>közlekedési csomópont</v>
       </c>
       <c r="H9" s="10">
@@ -10155,7 +10221,7 @@
         <v>80000000</v>
       </c>
       <c r="G10" t="str">
-        <f t="array" ref="G10">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A9))), "")</f>
+        <f t="array" ref="G10">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A9))), "")</f>
         <v/>
       </c>
       <c r="H10" s="10">
@@ -10189,7 +10255,7 @@
         <v/>
       </c>
       <c r="G11" t="str">
-        <f t="array" ref="G11">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A10))), "")</f>
+        <f t="array" ref="G11">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A10))), "")</f>
         <v/>
       </c>
       <c r="H11" s="10">
@@ -10223,7 +10289,7 @@
         <v>80000000</v>
       </c>
       <c r="G12" t="str">
-        <f t="array" ref="G12">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A11))), "")</f>
+        <f t="array" ref="G12">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A11))), "")</f>
         <v/>
       </c>
       <c r="H12" s="10">
@@ -10257,7 +10323,7 @@
         <v>80000000</v>
       </c>
       <c r="G13" t="str">
-        <f t="array" ref="G13">IFERROR(INDEX($E$2:$E$1000000, SMALL(IF($E$2:$E$1000000&lt;&gt;"", ROW($E$2:$E$1000000)-ROW($E$2)+1), ROW(A12))), "")</f>
+        <f t="array" ref="G13">IFERROR(INDEX($E$2:$E$1048576, SMALL(IF($E$2:$E$1048576&lt;&gt;"", ROW($E$2:$E$1048576)-ROW($E$2)+1), ROW(A12))), "")</f>
         <v/>
       </c>
       <c r="H13" s="10">
@@ -10331,7 +10397,7 @@
         <v/>
       </c>
       <c r="C2" t="str">
-        <f t="array" ref="C2">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A1))), "")</f>
+        <f t="array" ref="C2">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A1))), "")</f>
         <v>lakóház</v>
       </c>
       <c r="D2">
@@ -10350,7 +10416,7 @@
         <v/>
       </c>
       <c r="C3" t="str">
-        <f t="array" ref="C3">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A2))), "")</f>
+        <f t="array" ref="C3">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A2))), "")</f>
         <v>iskola</v>
       </c>
       <c r="D3">
@@ -10369,7 +10435,7 @@
         <v/>
       </c>
       <c r="C4" t="str">
-        <f t="array" ref="C4">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A3))), "")</f>
+        <f t="array" ref="C4">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A3))), "")</f>
         <v>kórház</v>
       </c>
       <c r="D4">
@@ -10388,7 +10454,7 @@
         <v/>
       </c>
       <c r="C5" t="str">
-        <f t="array" ref="C5">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A4))), "")</f>
+        <f t="array" ref="C5">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A4))), "")</f>
         <v>üzlet</v>
       </c>
       <c r="D5">
@@ -10407,7 +10473,7 @@
         <v/>
       </c>
       <c r="C6" t="str">
-        <f t="array" ref="C6">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A5))), "")</f>
+        <f t="array" ref="C6">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A5))), "")</f>
         <v>gyár</v>
       </c>
       <c r="D6">
@@ -10426,7 +10492,7 @@
         <v/>
       </c>
       <c r="C7" t="str">
-        <f t="array" ref="C7">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A6))), "")</f>
+        <f t="array" ref="C7">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A6))), "")</f>
         <v>közlekedési csomópont</v>
       </c>
       <c r="D7">
@@ -10445,7 +10511,7 @@
         <v/>
       </c>
       <c r="C8" t="str">
-        <f t="array" ref="C8">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A7))), "")</f>
+        <f t="array" ref="C8">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A7))), "")</f>
         <v>rendőrség</v>
       </c>
       <c r="D8">
@@ -10464,7 +10530,7 @@
         <v>lakóház</v>
       </c>
       <c r="C9" t="str">
-        <f t="array" ref="C9">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A8))), "")</f>
+        <f t="array" ref="C9">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A8))), "")</f>
         <v>tűzoltóság</v>
       </c>
       <c r="D9">
@@ -10483,7 +10549,7 @@
         <v/>
       </c>
       <c r="C10" t="str">
-        <f t="array" ref="C10">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A9))), "")</f>
+        <f t="array" ref="C10">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A9))), "")</f>
         <v>kulturális</v>
       </c>
       <c r="D10">
@@ -10502,7 +10568,7 @@
         <v>iskola</v>
       </c>
       <c r="C11" t="str">
-        <f t="array" ref="C11">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A10))), "")</f>
+        <f t="array" ref="C11">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A10))), "")</f>
         <v>adminisztráció</v>
       </c>
       <c r="D11">
@@ -10521,7 +10587,7 @@
         <v/>
       </c>
       <c r="C12" t="str">
-        <f t="array" ref="C12">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A11))), "")</f>
+        <f t="array" ref="C12">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A11))), "")</f>
         <v>kereskedelem</v>
       </c>
       <c r="D12">
@@ -10540,7 +10606,7 @@
         <v>kórház</v>
       </c>
       <c r="C13" t="str">
-        <f t="array" ref="C13">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A12))), "")</f>
+        <f t="array" ref="C13">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A12))), "")</f>
         <v>szórakozás</v>
       </c>
       <c r="D13">
@@ -10559,7 +10625,7 @@
         <v/>
       </c>
       <c r="C14" t="str">
-        <f t="array" ref="C14">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A13))), "")</f>
+        <f t="array" ref="C14">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A13))), "")</f>
         <v/>
       </c>
       <c r="D14" t="str">
@@ -10577,7 +10643,7 @@
         <v>üzlet</v>
       </c>
       <c r="C15" t="str">
-        <f t="array" ref="C15">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A14))), "")</f>
+        <f t="array" ref="C15">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A14))), "")</f>
         <v/>
       </c>
       <c r="D15" t="str">
@@ -10595,7 +10661,7 @@
         <v/>
       </c>
       <c r="C16" t="str">
-        <f t="array" ref="C16">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A15))), "")</f>
+        <f t="array" ref="C16">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A15))), "")</f>
         <v/>
       </c>
       <c r="D16" t="str">
@@ -10613,7 +10679,7 @@
         <v>gyár</v>
       </c>
       <c r="C17" t="str">
-        <f t="array" ref="C17">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A16))), "")</f>
+        <f t="array" ref="C17">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A16))), "")</f>
         <v/>
       </c>
       <c r="D17" t="str">
@@ -10631,7 +10697,7 @@
         <v>közlekedési csomópont</v>
       </c>
       <c r="C18" t="str">
-        <f t="array" ref="C18">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A17))), "")</f>
+        <f t="array" ref="C18">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A17))), "")</f>
         <v/>
       </c>
       <c r="D18" t="str">
@@ -10649,7 +10715,7 @@
         <v>rendőrség</v>
       </c>
       <c r="C19" t="str">
-        <f t="array" ref="C19">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A18))), "")</f>
+        <f t="array" ref="C19">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A18))), "")</f>
         <v/>
       </c>
       <c r="D19" t="str">
@@ -10667,7 +10733,7 @@
         <v>tűzoltóság</v>
       </c>
       <c r="C20" t="str">
-        <f t="array" ref="C20">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A19))), "")</f>
+        <f t="array" ref="C20">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A19))), "")</f>
         <v/>
       </c>
       <c r="D20" t="str">
@@ -10685,7 +10751,7 @@
         <v>kulturális</v>
       </c>
       <c r="C21" t="str">
-        <f t="array" ref="C21">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A20))), "")</f>
+        <f t="array" ref="C21">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A20))), "")</f>
         <v/>
       </c>
       <c r="D21" t="str">
@@ -10703,7 +10769,7 @@
         <v>adminisztráció</v>
       </c>
       <c r="C22" t="str">
-        <f t="array" ref="C22">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A21))), "")</f>
+        <f t="array" ref="C22">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A21))), "")</f>
         <v/>
       </c>
       <c r="D22" t="str">
@@ -10721,7 +10787,7 @@
         <v>kereskedelem</v>
       </c>
       <c r="C23" t="str">
-        <f t="array" ref="C23">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A22))), "")</f>
+        <f t="array" ref="C23">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A22))), "")</f>
         <v/>
       </c>
       <c r="D23" t="str">
@@ -10739,7 +10805,7 @@
         <v/>
       </c>
       <c r="C24" t="str">
-        <f t="array" ref="C24">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A23))), "")</f>
+        <f t="array" ref="C24">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A23))), "")</f>
         <v/>
       </c>
       <c r="D24" t="str">
@@ -10757,7 +10823,7 @@
         <v/>
       </c>
       <c r="C25" t="str">
-        <f t="array" ref="C25">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A24))), "")</f>
+        <f t="array" ref="C25">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A24))), "")</f>
         <v/>
       </c>
       <c r="D25" t="str">
@@ -10775,7 +10841,7 @@
         <v>szórakozás</v>
       </c>
       <c r="C26" t="str">
-        <f t="array" ref="C26">IFERROR(INDEX($B$2:$B$1000000, SMALL(IF($B$2:$B$1000000&lt;&gt;"", ROW($B$2:$B$1000000)-ROW($B$2)+1), ROW(A25))), "")</f>
+        <f t="array" ref="C26">IFERROR(INDEX($B$2:$B$1048576, SMALL(IF($B$2:$B$1048576&lt;&gt;"", ROW($B$2:$B$1048576)-ROW($B$2)+1), ROW(A25))), "")</f>
         <v/>
       </c>
       <c r="D26" t="str">
@@ -10797,7 +10863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CBBC241-0578-4987-91E1-CB11E89C13A3}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>